<commit_message>
Implemented integrate method for WaveEquation for Dirichlet boundary conditions
</commit_message>
<xml_diff>
--- a/src/main/ui/excel_data/ODE.xlsx
+++ b/src/main/ui/excel_data/ODE.xlsx
@@ -11,6 +11,17 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,809 +351,817 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>0</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.1269330365086785</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1256637061435917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.253866073017357</v>
+        <v>0.1269330365086785</v>
       </c>
       <c r="B3">
-        <v>0.2493430105796443</v>
+        <v>0.1256637061435917</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.3807991095260356</v>
+        <v>0.253866073017357</v>
       </c>
       <c r="B4">
-        <v>0.3690848480163404</v>
+        <v>0.2493430105796443</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.5077321460347141</v>
+        <v>0.3807991095260356</v>
       </c>
       <c r="B5">
-        <v>0.4829983311484647</v>
+        <v>0.3690848480163404</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.6346651825433925</v>
+        <v>0.5077321460347141</v>
       </c>
       <c r="B6">
-        <v>0.5892846103528742</v>
+        <v>0.4829983311484647</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.7615982190520711</v>
+        <v>0.6346651825433925</v>
       </c>
       <c r="B7">
-        <v>0.6862652799831509</v>
+        <v>0.5892846103528742</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.8885312555607496</v>
+        <v>0.7615982190520711</v>
       </c>
       <c r="B8">
-        <v>0.7724088826892093</v>
+        <v>0.6862652799831509</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>1.015464292069428</v>
+        <v>0.8885312555607496</v>
       </c>
       <c r="B9">
-        <v>0.8463550932224198</v>
+        <v>0.7724088826892093</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>1.142397328578107</v>
+        <v>1.015464292069428</v>
       </c>
       <c r="B10">
-        <v>0.9069361998309063</v>
+        <v>0.8463550932224198</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>1.269330365086785</v>
+        <v>1.142397328578107</v>
       </c>
       <c r="B11">
-        <v>0.9531955440244195</v>
+        <v>0.9069361998309063</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>1.396263401595464</v>
+        <v>1.269330365086785</v>
       </c>
       <c r="B12">
-        <v>0.9844026275196892</v>
+        <v>0.9531955440244195</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>1.523196438104142</v>
+        <v>1.396263401595464</v>
       </c>
       <c r="B13">
-        <v>1.000064647806939</v>
+        <v>0.9844026275196892</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>1.650129474612821</v>
+        <v>1.523196438104142</v>
       </c>
       <c r="B14">
-        <v>0.9999342801751986</v>
+        <v>1.000064647806939</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>1.777062511121499</v>
+        <v>1.650129474612821</v>
       </c>
       <c r="B15">
-        <v>0.9840135833075903</v>
+        <v>0.9999342801751986</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>1.903995547630178</v>
+        <v>1.777062511121499</v>
       </c>
       <c r="B16">
-        <v>0.9525539667719111</v>
+        <v>0.9840135833075903</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>2.030928584138856</v>
+        <v>1.903995547630178</v>
       </c>
       <c r="B17">
-        <v>0.9060522209198684</v>
+        <v>0.9525539667719111</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>2.157861620647535</v>
+        <v>2.030928584138856</v>
       </c>
       <c r="B18">
-        <v>0.8452426718882937</v>
+        <v>0.9060522209198684</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>2.284794657156213</v>
+        <v>2.157861620647535</v>
       </c>
       <c r="B19">
-        <v>0.7710855855855875</v>
+        <v>0.8452426718882937</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>2.411727693664892</v>
+        <v>2.284794657156213</v>
       </c>
       <c r="B20">
-        <v>0.6847520037803019</v>
+        <v>0.7710855855855875</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>2.53866073017357</v>
+        <v>2.411727693664892</v>
       </c>
       <c r="B21">
-        <v>0.5876052517507526</v>
+        <v>0.6847520037803019</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>2.665593766682249</v>
+        <v>2.53866073017357</v>
       </c>
       <c r="B22">
-        <v>0.4811794095151514</v>
+        <v>0.5876052517507526</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>2.792526803190927</v>
+        <v>2.665593766682249</v>
       </c>
       <c r="B23">
-        <v>0.3671550866109672</v>
+        <v>0.4811794095151514</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>2.919459839699606</v>
+        <v>2.792526803190927</v>
       </c>
       <c r="B24">
-        <v>0.2473328829728664</v>
+        <v>0.3671550866109672</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>3.046392876208285</v>
+        <v>2.919459839699606</v>
       </c>
       <c r="B25">
-        <v>0.1236049549982485</v>
+        <v>0.2473328829728664</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>3.173325912716963</v>
+        <v>3.046392876208285</v>
       </c>
       <c r="B26">
-        <v>-0.002074864188924774</v>
+        <v>0.1236049549982485</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>3.300258949225642</v>
+        <v>3.173325912716963</v>
       </c>
       <c r="B27">
-        <v>-0.127721918434129</v>
+        <v>-0.002074864188924774</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>3.42719198573432</v>
+        <v>3.300258949225642</v>
       </c>
       <c r="B28">
-        <v>-0.2513520689860643</v>
+        <v>-0.127721918434129</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>3.554125022242999</v>
+        <v>3.42719198573432</v>
       </c>
       <c r="B29">
-        <v>-0.3710130267599392</v>
+        <v>-0.2513520689860643</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>3.681058058751677</v>
+        <v>3.554125022242999</v>
       </c>
       <c r="B30">
-        <v>-0.4848151816509799</v>
+        <v>-0.3710130267599392</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>3.807991095260356</v>
+        <v>3.681058058751677</v>
       </c>
       <c r="B31">
-        <v>-0.5909614420611606</v>
+        <v>-0.4848151816509799</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>3.934924131769034</v>
+        <v>3.807991095260356</v>
       </c>
       <c r="B32">
-        <v>-0.6877756134322359</v>
+        <v>-0.5909614420611606</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>4.061857168277712</v>
+        <v>3.934924131769034</v>
       </c>
       <c r="B33">
-        <v>-0.7737288676492428</v>
+        <v>-0.6877756134322359</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>4.188790204786391</v>
+        <v>4.061857168277712</v>
       </c>
       <c r="B34">
-        <v>-0.8474638853264083</v>
+        <v>-0.7737288676492428</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>4.315723241295069</v>
+        <v>4.188790204786391</v>
       </c>
       <c r="B35">
-        <v>-0.9078162897357629</v>
+        <v>-0.8474638853264083</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>4.442656277803748</v>
+        <v>4.315723241295069</v>
       </c>
       <c r="B36">
-        <v>-0.9538330339074268</v>
+        <v>-0.9078162897357629</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>4.569589314312426</v>
+        <v>4.442656277803748</v>
       </c>
       <c r="B37">
-        <v>-0.9847874505441192</v>
+        <v>-0.9538330339074268</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>4.696522350821105</v>
+        <v>4.569589314312426</v>
       </c>
       <c r="B38">
-        <v>-1.000190727091167</v>
+        <v>-0.9847874505441192</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>4.823455387329783</v>
+        <v>4.696522350821105</v>
       </c>
       <c r="B39">
-        <v>-0.9997996247549708</v>
+        <v>-1.000190727091167</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>4.950388423838462</v>
+        <v>4.823455387329783</v>
       </c>
       <c r="B40">
-        <v>-0.9836203195760717</v>
+        <v>-0.9997996247549708</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>5.07732146034714</v>
+        <v>4.950388423838462</v>
       </c>
       <c r="B41">
-        <v>-0.9519083049010303</v>
+        <v>-0.9836203195760717</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>5.204254496855819</v>
+        <v>5.07732146034714</v>
       </c>
       <c r="B42">
-        <v>-0.9051643567932134</v>
+        <v>-0.9519083049010303</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>5.331187533364497</v>
+        <v>5.204254496855819</v>
       </c>
       <c r="B43">
-        <v>-0.8441266260941717</v>
+        <v>-0.9051643567932134</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>5.458120569873176</v>
+        <v>5.331187533364497</v>
       </c>
       <c r="B44">
-        <v>-0.7697589820127687</v>
+        <v>-0.8441266260941717</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>5.585053606381854</v>
+        <v>5.458120569873176</v>
       </c>
       <c r="B45">
-        <v>-0.6832357913127237</v>
+        <v>-0.7697589820127687</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>5.711986642890533</v>
+        <v>5.585053606381854</v>
       </c>
       <c r="B46">
-        <v>-0.5859233734560038</v>
+        <v>-0.6832357913127237</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>5.838919679399211</v>
+        <v>5.711986642890533</v>
       </c>
       <c r="B47">
-        <v>-0.4793584245507038</v>
+        <v>-0.5859233734560038</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>5.96585271590789</v>
+        <v>5.838919679399211</v>
       </c>
       <c r="B48">
-        <v>-0.3652237508187721</v>
+        <v>-0.4793584245507038</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>6.092785752416569</v>
+        <v>5.96585271590789</v>
       </c>
       <c r="B49">
-        <v>-0.245321694785299</v>
+        <v>-0.3652237508187721</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>6.219718788925247</v>
+        <v>6.092785752416569</v>
       </c>
       <c r="B50">
-        <v>-0.1215456738261689</v>
+        <v>-0.245321694785299</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>6.346651825433926</v>
+        <v>6.219718788925247</v>
       </c>
       <c r="B51">
-        <v>0.004149719480686306</v>
+        <v>-0.1215456738261689</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>6.473584861942604</v>
+        <v>6.346651825433926</v>
       </c>
       <c r="B52">
-        <v>0.1297795830441017</v>
+        <v>0.004149719480686306</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>6.600517898451283</v>
+        <v>6.473584861942604</v>
       </c>
       <c r="B53">
-        <v>0.2533600495771433</v>
+        <v>0.1297795830441017</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>6.727450934959961</v>
+        <v>6.600517898451283</v>
       </c>
       <c r="B54">
-        <v>0.372939614573598</v>
+        <v>0.2533600495771433</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>6.85438397146864</v>
+        <v>6.727450934959961</v>
       </c>
       <c r="B55">
-        <v>0.4866299532319149</v>
+        <v>0.372939614573598</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>6.981317007977318</v>
+        <v>6.85438397146864</v>
       </c>
       <c r="B56">
-        <v>0.5926357396852404</v>
+        <v>0.4866299532319149</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>7.108250044485997</v>
+        <v>6.981317007977318</v>
       </c>
       <c r="B57">
-        <v>0.6892829976511414</v>
+        <v>0.5926357396852404</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>7.235183080994675</v>
+        <v>7.108250044485997</v>
       </c>
       <c r="B58">
-        <v>0.7750455348055004</v>
+        <v>0.6892829976511414</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>7.362116117503354</v>
+        <v>7.235183080994675</v>
       </c>
       <c r="B59">
-        <v>0.8485690434456818</v>
+        <v>0.7750455348055004</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>7.489049154012032</v>
+        <v>7.362116117503354</v>
       </c>
       <c r="B60">
-        <v>0.9086924868605517</v>
+        <v>0.8485690434456818</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>7.615982190520711</v>
+        <v>7.489049154012032</v>
       </c>
       <c r="B61">
-        <v>0.9544664336873324</v>
+        <v>0.9086924868605517</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>7.742915227029389</v>
+        <v>7.615982190520711</v>
       </c>
       <c r="B62">
-        <v>0.985168050730733</v>
+        <v>0.9544664336873324</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>7.869848263538068</v>
+        <v>7.742915227029389</v>
       </c>
       <c r="B63">
-        <v>1.000312517487246</v>
+        <v>0.985168050730733</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>7.996781300046746</v>
+        <v>7.869848263538068</v>
       </c>
       <c r="B64">
-        <v>0.9996606821236681</v>
+        <v>1.000312517487246</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>8.123714336555425</v>
+        <v>7.996781300046746</v>
       </c>
       <c r="B65">
-        <v>0.9832228380114761</v>
+        <v>0.9996606821236681</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>8.250647373064103</v>
+        <v>8.123714336555425</v>
       </c>
       <c r="B66">
-        <v>0.9512585611804208</v>
+        <v>0.9832228380114761</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>8.377580409572783</v>
+        <v>8.250647373064103</v>
       </c>
       <c r="B67">
-        <v>0.9042726112581652</v>
+        <v>0.9512585611804208</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>8.504513446081461</v>
+        <v>8.377580409572783</v>
       </c>
       <c r="B68">
-        <v>0.8430069606257364</v>
+        <v>0.9042726112581652</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>8.631446482590139</v>
+        <v>8.504513446081461</v>
       </c>
       <c r="B69">
-        <v>0.7684290776593226</v>
+        <v>0.8430069606257364</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>8.758379519098817</v>
+        <v>8.631446482590139</v>
       </c>
       <c r="B70">
-        <v>0.6817166490820423</v>
+        <v>0.7684290776593226</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>8.885312555607497</v>
+        <v>8.758379519098817</v>
       </c>
       <c r="B71">
-        <v>0.5842389826806405</v>
+        <v>0.6817166490820423</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>9.012245592116175</v>
+        <v>8.885312555607497</v>
       </c>
       <c r="B72">
-        <v>0.477535384063634</v>
+        <v>0.5842389826806405</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>9.139178628624853</v>
+        <v>9.012245592116175</v>
       </c>
       <c r="B73">
-        <v>0.3632908489214591</v>
+        <v>0.477535384063634</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>9.266111665133531</v>
+        <v>9.139178628624853</v>
       </c>
       <c r="B74">
-        <v>0.243309454641059</v>
+        <v>0.3632908489214591</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>9.393044701642211</v>
+        <v>9.266111665133531</v>
       </c>
       <c r="B75">
-        <v>0.1194858714576956</v>
+        <v>0.243309454641059</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>9.519977738150889</v>
+        <v>9.393044701642211</v>
       </c>
       <c r="B76">
-        <v>-0.006224556978158782</v>
+        <v>0.1194858714576956</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>9.646910774659567</v>
+        <v>9.519977738150889</v>
       </c>
       <c r="B77">
-        <v>-0.1318366911500988</v>
+        <v>-0.006224556978158782</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>9.773843811168245</v>
+        <v>9.646910774659567</v>
       </c>
       <c r="B78">
-        <v>-0.2553669437425187</v>
+        <v>-0.1318366911500988</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>9.900776847676925</v>
+        <v>9.773843811168245</v>
       </c>
       <c r="B79">
-        <v>-0.3748646031959724</v>
+        <v>-0.2553669437425187</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>10.0277098841856</v>
+        <v>9.900776847676925</v>
       </c>
       <c r="B80">
-        <v>-0.4884426381094011</v>
+        <v>-0.3748646031959724</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>10.15464292069428</v>
+        <v>10.0277098841856</v>
       </c>
       <c r="B81">
-        <v>-0.5943074960456071</v>
+        <v>-0.4884426381094011</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>10.28157595720296</v>
+        <v>10.15464292069428</v>
       </c>
       <c r="B82">
-        <v>-0.6907874261760976</v>
+        <v>-0.5943074960456071</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>10.40850899371164</v>
+        <v>10.28157595720296</v>
       </c>
       <c r="B83">
-        <v>-0.7763588785120205</v>
+        <v>-0.6907874261760976</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>10.53544203022032</v>
+        <v>10.40850899371164</v>
       </c>
       <c r="B84">
-        <v>-0.8496705628412441</v>
+        <v>-0.7763588785120205</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>10.66237506672899</v>
+        <v>10.53544203022032</v>
       </c>
       <c r="B85">
-        <v>-0.9095647874480772</v>
+        <v>-0.8496705628412441</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>10.78930810323767</v>
+        <v>10.66237506672899</v>
       </c>
       <c r="B86">
-        <v>-0.9550957406480729</v>
+        <v>-0.9095647874480772</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>10.91624113974635</v>
+        <v>10.78930810323767</v>
       </c>
       <c r="B87">
-        <v>-0.9855444264474895</v>
+        <v>-0.9550957406480729</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>11.04317417625503</v>
+        <v>10.91624113974635</v>
       </c>
       <c r="B88">
-        <v>-1.00043001847293</v>
+        <v>-0.9855444264474895</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>11.17010721276371</v>
+        <v>11.04317417625503</v>
       </c>
       <c r="B89">
-        <v>-0.9995174528770863</v>
+        <v>-1.00043001847293</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>11.29704024927239</v>
+        <v>11.17010721276371</v>
       </c>
       <c r="B90">
-        <v>-0.9828211403182326</v>
+        <v>-0.9995174528770863</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>11.42397328578107</v>
+        <v>11.29704024927239</v>
       </c>
       <c r="B91">
-        <v>-0.9506047383962294</v>
+        <v>-0.9828211403182326</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>11.55090632228974</v>
+        <v>11.42397328578107</v>
       </c>
       <c r="B92">
-        <v>-0.9033769881385912</v>
+        <v>-0.9506047383962294</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>11.67783935879842</v>
+        <v>11.55090632228974</v>
       </c>
       <c r="B93">
-        <v>-0.8418836802841924</v>
+        <v>-0.9033769881385912</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>11.8047723953071</v>
+        <v>11.67783935879842</v>
       </c>
       <c r="B94">
-        <v>-0.7670958782279723</v>
+        <v>-0.8418836802841924</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>11.93170543181578</v>
+        <v>11.8047723953071</v>
       </c>
       <c r="B95">
-        <v>-0.6801945836024462</v>
+        <v>-0.7670958782279723</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>12.05863846832446</v>
+        <v>11.93170543181578</v>
       </c>
       <c r="B96">
-        <v>-0.5825520866474484</v>
+        <v>-0.6801945836024462</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>12.18557150483314</v>
+        <v>12.05863846832446</v>
       </c>
       <c r="B97">
-        <v>-0.4757102958712675</v>
+        <v>-0.5825520866474484</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>12.31250454134182</v>
+        <v>12.18557150483314</v>
       </c>
       <c r="B98">
-        <v>-0.3613563892074472</v>
+        <v>-0.4757102958712675</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>12.43943757785049</v>
+        <v>12.31250454134182</v>
       </c>
       <c r="B99">
-        <v>-0.2412961711687732</v>
+        <v>-0.3613563892074472</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
+        <v>12.43943757785049</v>
+      </c>
+      <c r="B100">
+        <v>-0.2412961711687732</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101">
         <v>12.56637061435917</v>
       </c>
-      <c r="B100">
+      <c r="B101">
         <v>-0.1174255567254058</v>
       </c>
     </row>

</xml_diff>